<commit_message>
prismify needs template schema and instance only
</commit_message>
<xml_diff>
--- a/tests/data/tiny_manifest.xlsx
+++ b/tests/data/tiny_manifest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jlurye/code/cidc-schemas/tests/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39CBB937-3010-0C4C-BF89-DE8D4A41B3BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3555403E-7104-E848-8DE7-2644E0292AB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3520" yWindow="7340" windowWidth="28040" windowHeight="9560" xr2:uid="{C0BBF449-F049-8243-B3CC-F67B2B5BF66B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>#p</t>
   </si>
@@ -52,6 +52,9 @@
   </si>
   <si>
     <t>#d</t>
+  </si>
+  <si>
+    <t>test_number</t>
   </si>
 </sst>
 </file>
@@ -408,10 +411,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC495060-BC08-7247-8F05-1DB3ED750A59}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M6" sqref="M6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -419,7 +422,7 @@
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -430,7 +433,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -441,7 +444,7 @@
         <v>41071</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -452,32 +455,49 @@
         <v>0.44792824074074072</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4">
+        <v>1.2344999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>5</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B7" t="s">
         <v>1</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D7" t="s">
         <v>4</v>
       </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>6</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B8" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C8" s="1">
         <v>41071</v>
       </c>
-      <c r="D6" s="2">
+      <c r="D8" s="2">
         <v>0.44792824074074072</v>
+      </c>
+      <c r="E8">
+        <v>1.2344999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test for enum validation through Data Dict sheet in template writer
</commit_message>
<xml_diff>
--- a/tests/data/tiny_manifest.xlsx
+++ b/tests/data/tiny_manifest.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pavel/code/cidc-schemas/tests/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3555403E-7104-E848-8DE7-2644E0292AB9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06E8B3C8-0569-9D43-B0AE-61EFC8095594}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3520" yWindow="7340" windowWidth="28040" windowHeight="9560" xr2:uid="{C0BBF449-F049-8243-B3CC-F67B2B5BF66B}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="10">
   <si>
     <t>#p</t>
   </si>
@@ -55,6 +55,12 @@
   </si>
   <si>
     <t>test_number</t>
+  </si>
+  <si>
+    <t>test_enum</t>
+  </si>
+  <si>
+    <t>enum_val_1</t>
   </si>
 </sst>
 </file>
@@ -411,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC495060-BC08-7247-8F05-1DB3ED750A59}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -422,7 +428,7 @@
     <col min="3" max="3" width="11.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -433,7 +439,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -444,7 +450,7 @@
         <v>41071</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>0</v>
       </c>
@@ -455,7 +461,7 @@
         <v>0.44792824074074072</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>0</v>
       </c>
@@ -466,7 +472,18 @@
         <v>1.2344999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -482,8 +499,11 @@
       <c r="E7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -498,6 +518,9 @@
       </c>
       <c r="E8">
         <v>1.2344999999999999</v>
+      </c>
+      <c r="F8" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>